<commit_message>
[new Update] Vishal appium
</commit_message>
<xml_diff>
--- a/TestData/NaukariLoginDetails.xlsx
+++ b/TestData/NaukariLoginDetails.xlsx
@@ -32,7 +32,7 @@
     <t>vchapde@123</t>
   </si>
   <si>
-    <t>Software Test Engineer with 3.1 years of experience in software quality processes, Involved in end-to-end features testing. Skills in Automation testing, Manual UI Testing, Database and API Testing. Working knowledge of Cucumber for BDD.</t>
+    <t>Software Test Engineer with 3.2 years of experience in software quality processes, Involved in end-to-end features testing. Skills in Automation, Manual UI Testing, Mobile Testing, Database and API Testing.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>